<commit_message>
doplneni legend do exportu, formatovani, detail, focused_rámeček
</commit_message>
<xml_diff>
--- a/catalogue_manager/Katalog_kamerového_vybavení.xlsx
+++ b/catalogue_manager/Katalog_kamerového_vybavení.xlsx
@@ -42,7 +42,7 @@
       <sz val="16"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -51,14 +51,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00757575"/>
-        <bgColor rgb="00757575"/>
+        <fgColor rgb="0032CD32"/>
+        <bgColor rgb="0032CD32"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00999999"/>
+        <bgColor rgb="00999999"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00636363"/>
         <bgColor rgb="00636363"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001E90FF"/>
+        <bgColor rgb="001E90FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -80,16 +92,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -97,8 +109,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -174,21 +198,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>TRIMAZKON</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
-      <text>
-        <t>Pravým klikem na buňky v tabulce zobrazíte podrobnosti</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -510,7 +519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +535,7 @@
     <col width="50" customWidth="1" min="6" max="6"/>
     <col width="50" customWidth="1" min="7" max="7"/>
     <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="50" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="35" customHeight="1">
@@ -539,7 +549,7 @@
       <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Projekt: 
-Datum: 03.07.2024</t>
+Datum: 06.07.2024</t>
         </is>
       </c>
     </row>
@@ -568,6 +578,11 @@
         </is>
       </c>
       <c r="H3" s="3" t="n"/>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>Legenda kontrolerů</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
@@ -575,202 +590,53 @@
           <t>Název stanice</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>- popis inspekce</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>Typ kamery</t>
-        </is>
-      </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Kontroler: 
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- popis inspekce
 </t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>Objektiv</t>
-        </is>
-      </c>
+      <c r="C4" s="6" t="inlineStr"/>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kontroler: Kontroler 2  (FH-2050)
+</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr"/>
       <c r="F4" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alternativa: 
+          <t>
 </t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr"/>
       <c r="H4" s="4" t="inlineStr"/>
+      <c r="I4" s="8" t="inlineStr">
+        <is>
+          <t>Kontroler 1  (FH-2050)</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="n"/>
-      <c r="B5" s="6" t="n"/>
-      <c r="C5" s="6" t="n"/>
-      <c r="D5" s="6" t="n"/>
-      <c r="E5" s="6" t="n"/>
-      <c r="F5" s="6" t="n"/>
-      <c r="G5" s="6" t="n"/>
-      <c r="H5" s="6" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Název stanice</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">- popis inspekce
-</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>FH-SC</t>
-        </is>
-      </c>
-      <c r="D6" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Kontroler: Kontroler 1 (FH-2050)
-IPadresa:192.168.000.000xz
-Jméno:zc
-Heslo:zc
-</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t>3Z4S-LE SV-0814H</t>
-        </is>
-      </c>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Alternativa: 
-</t>
-        </is>
-      </c>
-      <c r="G6" s="4" t="inlineStr"/>
-      <c r="H6" s="4" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="n"/>
-      <c r="B7" s="6" t="n"/>
-      <c r="C7" s="6" t="n"/>
-      <c r="D7" s="6" t="n"/>
-      <c r="E7" s="6" t="n"/>
-      <c r="F7" s="6" t="n"/>
-      <c r="G7" s="6" t="n"/>
-      <c r="H7" s="6" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>Název stanice</t>
-        </is>
-      </c>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>- popis inspekce</t>
-        </is>
-      </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>Typ kamery</t>
-        </is>
-      </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Kontroler: 
-</t>
-        </is>
-      </c>
-      <c r="E8" s="4" t="inlineStr">
-        <is>
-          <t>Objektiv</t>
-        </is>
-      </c>
-      <c r="F8" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Alternativa: 
-</t>
-        </is>
-      </c>
-      <c r="G8" s="4" t="inlineStr"/>
-      <c r="H8" s="4" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="n"/>
-      <c r="B9" s="6" t="n"/>
-      <c r="C9" s="6" t="n"/>
-      <c r="D9" s="6" t="n"/>
-      <c r="E9" s="6" t="n"/>
-      <c r="F9" s="6" t="n"/>
-      <c r="G9" s="6" t="n"/>
-      <c r="H9" s="6" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Název stanice</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>- popis inspekce</t>
-        </is>
-      </c>
-      <c r="C10" s="4" t="inlineStr">
-        <is>
-          <t>Typ kamery</t>
-        </is>
-      </c>
-      <c r="D10" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Kontroler: 
-</t>
-        </is>
-      </c>
-      <c r="E10" s="4" t="inlineStr">
-        <is>
-          <t>Objektiv</t>
-        </is>
-      </c>
-      <c r="F10" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Alternativa: 
-</t>
-        </is>
-      </c>
-      <c r="G10" s="4" t="inlineStr"/>
-      <c r="H10" s="4" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="n"/>
-      <c r="B11" s="6" t="n"/>
-      <c r="C11" s="6" t="n"/>
-      <c r="D11" s="6" t="n"/>
-      <c r="E11" s="6" t="n"/>
-      <c r="F11" s="6" t="n"/>
-      <c r="G11" s="6" t="n"/>
-      <c r="H11" s="6" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="n"/>
-      <c r="B12" s="4" t="n"/>
-      <c r="C12" s="4" t="n"/>
-      <c r="D12" s="4" t="n"/>
-      <c r="E12" s="4" t="n"/>
-      <c r="F12" s="4" t="n"/>
-      <c r="G12" s="4" t="n"/>
-      <c r="H12" s="4" t="n"/>
+      <c r="A5" s="9" t="n"/>
+      <c r="B5" s="9" t="n"/>
+      <c r="C5" s="9" t="n"/>
+      <c r="D5" s="9" t="n"/>
+      <c r="E5" s="9" t="n"/>
+      <c r="F5" s="9" t="n"/>
+      <c r="G5" s="9" t="n"/>
+      <c r="H5" s="9" t="n"/>
+      <c r="I5" s="10" t="inlineStr">
+        <is>
+          <t>Kontroler 2  (FH-2050)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:H3"/>
@@ -779,6 +645,5 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
plně funkční ukládání rozpracovaného projektu do xml, kompletní navigátor při přidávání nové stanice
</commit_message>
<xml_diff>
--- a/catalogue_manager/Katalog_kamerového_vybavení.xlsx
+++ b/catalogue_manager/Katalog_kamerového_vybavení.xlsx
@@ -92,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -109,20 +109,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,7 +522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,7 +552,7 @@
       <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Projekt: 
-Datum: 06.07.2024</t>
+Datum: 07.07.2024</t>
         </is>
       </c>
     </row>
@@ -596,42 +599,83 @@
 </t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr"/>
-      <c r="D4" s="7" t="inlineStr">
+      <c r="C4" s="4" t="inlineStr"/>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr"/>
+      <c r="H4" s="4" t="inlineStr"/>
+      <c r="I4" s="6" t="inlineStr">
+        <is>
+          <t>Kontroler 1  (FH-2050)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="n"/>
+      <c r="B5" s="7" t="n"/>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="G5" s="7" t="n"/>
+      <c r="H5" s="7" t="n"/>
+      <c r="I5" s="8" t="inlineStr">
+        <is>
+          <t>Kontroler 2  (FH-2050)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Název stanice</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- popis inspekce
+</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr"/>
+      <c r="D6" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">Kontroler: Kontroler 2  (FH-2050)
 </t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="E6" s="4" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>
 </t>
         </is>
       </c>
-      <c r="G4" s="4" t="inlineStr"/>
-      <c r="H4" s="4" t="inlineStr"/>
-      <c r="I4" s="8" t="inlineStr">
-        <is>
-          <t>Kontroler 1  (FH-2050)</t>
-        </is>
-      </c>
+      <c r="G6" s="4" t="inlineStr"/>
+      <c r="H6" s="4" t="inlineStr"/>
+      <c r="I6" s="11" t="n"/>
     </row>
-    <row r="5">
-      <c r="A5" s="9" t="n"/>
-      <c r="B5" s="9" t="n"/>
-      <c r="C5" s="9" t="n"/>
-      <c r="D5" s="9" t="n"/>
-      <c r="E5" s="9" t="n"/>
-      <c r="F5" s="9" t="n"/>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="9" t="n"/>
-      <c r="I5" s="10" t="inlineStr">
-        <is>
-          <t>Kontroler 2  (FH-2050)</t>
-        </is>
-      </c>
+    <row r="7">
+      <c r="A7" s="7" t="n"/>
+      <c r="B7" s="7" t="n"/>
+      <c r="C7" s="7" t="n"/>
+      <c r="D7" s="7" t="n"/>
+      <c r="E7" s="7" t="n"/>
+      <c r="F7" s="7" t="n"/>
+      <c r="G7" s="7" t="n"/>
+      <c r="H7" s="7" t="n"/>
+      <c r="I7" s="11" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>